<commit_message>
MAJ tableau de competences
</commit_message>
<xml_diff>
--- a/tools/Tableau de synthèse.xlsx
+++ b/tools/Tableau de synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Sources\2eme annee\epreuveE4\DanTOUATI.github.Io\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E61BA9F-4EF3-4817-AC25-4E4B01A3D72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76B21BCD-9E4E-4AD4-AB93-8E3FC416A45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,19 +145,19 @@
     <t>NOM et prénom : TOUATI Dan</t>
   </si>
   <si>
-    <t xml:space="preserve">création de site internet </t>
-  </si>
-  <si>
-    <t>Modifications d'un site internet</t>
-  </si>
-  <si>
-    <t>Maquettage/prototype d'applications</t>
-  </si>
-  <si>
     <t>X SLAM</t>
   </si>
   <si>
     <t>PORTFOLIO</t>
+  </si>
+  <si>
+    <t>CREATION D'UN SITE INTERNET</t>
+  </si>
+  <si>
+    <t>MODIFICATION D'UN SITE INTERNET</t>
+  </si>
+  <si>
+    <t>MAQUETTAGE/PROTOTYPE D'APPLICATION</t>
   </si>
 </sst>
 </file>
@@ -649,15 +649,39 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,30 +713,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1059,8 +1059,8 @@
   </sheetPr>
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1073,56 +1073,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="40" t="s">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="41"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="28"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1130,26 +1130,26 @@
         <v>5</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="37" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1172,8 +1172,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
@@ -1229,16 +1229,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="33"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13"/>
@@ -1480,16 +1480,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="36"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1528,7 +1528,7 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="13"/>
@@ -1578,16 +1578,16 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="36"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="13"/>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="13"/>
@@ -1817,11 +1817,6 @@
     <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -1829,6 +1824,11 @@
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1839,6 +1839,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2F8F9288E27CF4399AB296C013D9D54" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b5b11f149281ed3d8bc7f9ae8f827b95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2dc13c75-7b40-4bb0-99f5-7491ba72a134" xmlns:ns3="2b0f8d03-32c2-49cd-8e77-a752ab409d1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6df89cbc04f86a0c0fe9b9fced18d459" ns2:_="" ns3:_="">
     <xsd:import namespace="2dc13c75-7b40-4bb0-99f5-7491ba72a134"/>
@@ -2061,15 +2070,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2077,6 +2077,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63EFF976-E52E-425F-9A3D-717F0B4D1E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4217B69-E62E-4D99-8991-1807CD547B2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2095,14 +2103,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63EFF976-E52E-425F-9A3D-717F0B4D1E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0411A7-8762-454D-9B25-FAA96D916885}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
modif tableau de synth
</commit_message>
<xml_diff>
--- a/tools/Tableau de synthèse.xlsx
+++ b/tools/Tableau de synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Sources\2eme annee\epreuveE4\DanTOUATI.github.Io\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76B21BCD-9E4E-4AD4-AB93-8E3FC416A45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3AF3D0-FF29-413B-9068-81541BD801AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">N° candidat : </t>
-  </si>
-  <si>
     <t>Option :</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>MAQUETTAGE/PROTOTYPE D'APPLICATION</t>
+  </si>
+  <si>
+    <t>N° candidat : 02144624561</t>
   </si>
 </sst>
 </file>
@@ -649,9 +649,48 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -674,45 +713,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1059,8 +1059,8 @@
   </sheetPr>
   <dimension ref="A1:AQ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1073,124 +1073,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="28"/>
+      <c r="A3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="41"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
+      <c r="A4" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="H4" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="A5" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="30"/>
-      <c r="B7" s="38"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="30"/>
       <c r="C7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="F7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="H7" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>19</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -1229,16 +1229,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="33"/>
+      <c r="A8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="12"/>
@@ -1324,21 +1324,21 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10"/>
@@ -1379,12 +1379,12 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="13"/>
       <c r="D11" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="18"/>
@@ -1428,20 +1428,20 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1480,16 +1480,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
+      <c r="A13" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1528,18 +1528,18 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="13"/>
       <c r="H14" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1578,16 +1578,16 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="A15" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="28"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1626,13 +1626,13 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1675,16 +1675,16 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
@@ -1817,6 +1817,11 @@
     <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -1824,11 +1829,6 @@
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1839,15 +1839,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2F8F9288E27CF4399AB296C013D9D54" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b5b11f149281ed3d8bc7f9ae8f827b95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2dc13c75-7b40-4bb0-99f5-7491ba72a134" xmlns:ns3="2b0f8d03-32c2-49cd-8e77-a752ab409d1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6df89cbc04f86a0c0fe9b9fced18d459" ns2:_="" ns3:_="">
     <xsd:import namespace="2dc13c75-7b40-4bb0-99f5-7491ba72a134"/>
@@ -2070,6 +2061,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2077,14 +2077,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63EFF976-E52E-425F-9A3D-717F0B4D1E93}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4217B69-E62E-4D99-8991-1807CD547B2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2103,6 +2095,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63EFF976-E52E-425F-9A3D-717F0B4D1E93}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C0411A7-8762-454D-9B25-FAA96D916885}">
   <ds:schemaRefs>

</xml_diff>